<commit_message>
Update : correction des impacts et ajout des incertitudes
</commit_message>
<xml_diff>
--- a/Modele3/Database projet.xlsx
+++ b/Modele3/Database projet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dagos\Desktop\Unif\2020-2021\Q2\LBIR2130\Git\Modele\Modele3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C87968D-50E3-46D1-BB18-F876DFE64ECB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53733EB5-B17C-44F3-AB2D-EEDA3FC136E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="766" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -160,9 +160,6 @@
     <t>units2</t>
   </si>
   <si>
-    <t>certitude</t>
-  </si>
-  <si>
     <t xml:space="preserve">Quantité eau </t>
   </si>
   <si>
@@ -266,6 +263,9 @@
   </si>
   <si>
     <t>Sytra</t>
+  </si>
+  <si>
+    <t>incertitude</t>
   </si>
 </sst>
 </file>
@@ -1112,7 +1112,7 @@
         <v>36</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -4891,27 +4891,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -6390,13 +6390,14 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -6413,7 +6414,7 @@
         <v>38</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>39</v>
+        <v>74</v>
       </c>
       <c r="F1" s="21"/>
       <c r="G1" s="21"/>
@@ -6425,10 +6426,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="21" t="s">
         <v>40</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>41</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>35</v>
@@ -6442,10 +6443,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="21" t="s">
         <v>42</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>43</v>
       </c>
       <c r="D3" s="21" t="s">
         <v>35</v>
@@ -6459,10 +6460,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="21" t="s">
         <v>44</v>
-      </c>
-      <c r="C4" s="21" t="s">
-        <v>45</v>
       </c>
       <c r="D4" s="21" t="s">
         <v>35</v>
@@ -6476,10 +6477,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="21" t="s">
         <v>46</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>47</v>
       </c>
       <c r="D5" s="21" t="s">
         <v>35</v>
@@ -6493,13 +6494,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="D6" s="21" t="s">
         <v>49</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>50</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -6510,13 +6511,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="21" t="s">
-        <v>52</v>
-      </c>
       <c r="D7" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -6527,13 +6528,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="21" t="s">
-        <v>54</v>
-      </c>
       <c r="D8" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -6544,13 +6545,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E9">
         <v>2</v>
@@ -6561,13 +6562,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="21" t="s">
-        <v>57</v>
-      </c>
       <c r="D10" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -6578,10 +6579,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="21" t="s">
         <v>58</v>
-      </c>
-      <c r="C11" s="21" t="s">
-        <v>59</v>
       </c>
       <c r="D11" s="21" t="s">
         <v>35</v>
@@ -6595,10 +6596,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="21" t="s">
         <v>60</v>
-      </c>
-      <c r="C12" s="21" t="s">
-        <v>61</v>
       </c>
       <c r="D12" s="21" t="s">
         <v>35</v>
@@ -6612,10 +6613,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="21" t="s">
         <v>62</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>63</v>
       </c>
       <c r="D13" s="21" t="s">
         <v>35</v>
@@ -6629,10 +6630,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" t="s">
         <v>64</v>
-      </c>
-      <c r="C14" t="s">
-        <v>65</v>
       </c>
       <c r="D14" t="s">
         <v>35</v>
@@ -6643,13 +6644,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -6657,13 +6658,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" t="s">
         <v>67</v>
-      </c>
-      <c r="C16" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" t="s">
-        <v>68</v>
       </c>
       <c r="E16">
         <v>1.2199999999999999E-3</v>
@@ -6833,18 +6834,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6866,18 +6867,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACB07B5E-BECD-4F33-B1FB-15593DB46C88}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E5C67A9-63B7-498A-88A5-7B4488417ED6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACB07B5E-BECD-4F33-B1FB-15593DB46C88}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>